<commit_message>
2023, uppdat 9 - korrigering
2023, uppdat 9 - korrigering
</commit_message>
<xml_diff>
--- a/Bibsam_tidskriftslistor/scifree_data_gruyter_fullyoa.xlsx
+++ b/Bibsam_tidskriftslistor/scifree_data_gruyter_fullyoa.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_2A830853D38270106A6CB1D9A84071AE7AE981AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7EA6B4D-7E5D-4B0F-8839-A6BB93BDE0B3}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_2A830853D38270106A6CB1D9A84071AE7AE981AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DFB6BDC-4F98-4474-B723-EE972AD89F94}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="341">
   <si>
     <t>Open</t>
   </si>
@@ -791,15 +791,6 @@
   </si>
   <si>
     <t>http://www.degruyter.com/view/j/crpm</t>
-  </si>
-  <si>
-    <t>2329-8766</t>
-  </si>
-  <si>
-    <t>Energy Harvesting and Systems</t>
-  </si>
-  <si>
-    <t>http://www.degruyter.com/view/j/ehs</t>
   </si>
   <si>
     <t>2169-0375</t>
@@ -1105,23 +1096,6 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1140,6 +1114,23 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1154,10 +1145,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G112" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:G112" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G106">
-    <sortCondition ref="D1:D106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G111" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:G111" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G105">
+    <sortCondition ref="D1:D105"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Imprint"/>
@@ -1435,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,13 +1471,13 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1589,13 +1580,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -1718,13 +1709,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E13" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
@@ -1738,13 +1729,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D14" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F14" t="s">
         <v>0</v>
@@ -1758,13 +1749,13 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D15" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E15" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
@@ -1778,13 +1769,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E16" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -1959,13 +1950,13 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E24" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F24" t="s">
         <v>0</v>
@@ -1979,13 +1970,13 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D25" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E25" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F25" t="s">
         <v>0</v>
@@ -1999,13 +1990,13 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D26" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E26" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F26" t="s">
         <v>0</v>
@@ -2042,13 +2033,16 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>258</v>
+        <v>106</v>
       </c>
       <c r="E28" t="s">
-        <v>259</v>
+        <v>177</v>
       </c>
       <c r="F28" t="s">
         <v>0</v>
@@ -2062,16 +2056,16 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F29" t="s">
         <v>0</v>
@@ -2085,16 +2079,16 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F30" t="s">
         <v>0</v>
@@ -2108,16 +2102,16 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E31" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F31" t="s">
         <v>0</v>
@@ -2131,16 +2125,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>236</v>
       </c>
       <c r="E32" t="s">
-        <v>182</v>
+        <v>245</v>
       </c>
       <c r="F32" t="s">
         <v>0</v>
@@ -2154,13 +2145,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>227</v>
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>236</v>
+        <v>112</v>
       </c>
       <c r="E33" t="s">
-        <v>245</v>
+        <v>183</v>
       </c>
       <c r="F33" t="s">
         <v>0</v>
@@ -2174,16 +2168,13 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
+        <v>268</v>
       </c>
       <c r="D34" t="s">
-        <v>112</v>
+        <v>285</v>
       </c>
       <c r="E34" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="F34" t="s">
         <v>0</v>
@@ -2197,13 +2188,13 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="D35" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="E35" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="F35" t="s">
         <v>0</v>
@@ -2217,10 +2208,10 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>228</v>
+        <v>269</v>
       </c>
       <c r="D36" t="s">
-        <v>237</v>
+        <v>286</v>
       </c>
       <c r="E36" t="s">
         <v>246</v>
@@ -2237,13 +2228,13 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D37" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E37" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
       <c r="F37" t="s">
         <v>0</v>
@@ -2257,13 +2248,16 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>273</v>
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>290</v>
+        <v>115</v>
       </c>
       <c r="E38" t="s">
-        <v>306</v>
+        <v>186</v>
       </c>
       <c r="F38" t="s">
         <v>0</v>
@@ -2277,16 +2271,16 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E39" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F39" t="s">
         <v>0</v>
@@ -2300,16 +2294,13 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>33</v>
+        <v>229</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>238</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>247</v>
       </c>
       <c r="F40" t="s">
         <v>0</v>
@@ -2323,13 +2314,13 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E41" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F41" t="s">
         <v>0</v>
@@ -2343,13 +2334,13 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D42" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E42" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F42" t="s">
         <v>0</v>
@@ -2363,13 +2354,13 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D43" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E43" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F43" t="s">
         <v>0</v>
@@ -2383,13 +2374,13 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="D44" t="s">
-        <v>241</v>
+        <v>288</v>
       </c>
       <c r="E44" t="s">
-        <v>250</v>
+        <v>304</v>
       </c>
       <c r="F44" t="s">
         <v>0</v>
@@ -2403,13 +2394,16 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>274</v>
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>291</v>
+        <v>114</v>
       </c>
       <c r="E45" t="s">
-        <v>307</v>
+        <v>185</v>
       </c>
       <c r="F45" t="s">
         <v>0</v>
@@ -2423,16 +2417,16 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
         <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E46" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F46" t="s">
         <v>0</v>
@@ -2446,16 +2440,13 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" t="s">
-        <v>33</v>
+        <v>272</v>
       </c>
       <c r="D47" t="s">
-        <v>116</v>
+        <v>289</v>
       </c>
       <c r="E47" t="s">
-        <v>187</v>
+        <v>305</v>
       </c>
       <c r="F47" t="s">
         <v>0</v>
@@ -2469,13 +2460,13 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="D48" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E48" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F48" t="s">
         <v>0</v>
@@ -2489,13 +2480,16 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>313</v>
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
       </c>
       <c r="D49" t="s">
-        <v>293</v>
+        <v>119</v>
       </c>
       <c r="E49" t="s">
-        <v>309</v>
+        <v>190</v>
       </c>
       <c r="F49" t="s">
         <v>0</v>
@@ -2509,16 +2503,16 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
         <v>33</v>
       </c>
       <c r="D50" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E50" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F50" t="s">
         <v>0</v>
@@ -2532,16 +2526,16 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C51" t="s">
         <v>33</v>
       </c>
       <c r="D51" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E51" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F51" t="s">
         <v>0</v>
@@ -2555,16 +2549,16 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
         <v>33</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E52" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F52" t="s">
         <v>0</v>
@@ -2578,16 +2572,16 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
         <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E53" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F53" t="s">
         <v>0</v>
@@ -2601,16 +2595,16 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s">
         <v>33</v>
       </c>
       <c r="D54" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E54" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F54" t="s">
         <v>0</v>
@@ -2624,16 +2618,16 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
         <v>33</v>
       </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E55" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F55" t="s">
         <v>0</v>
@@ -2647,16 +2641,16 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
         <v>33</v>
       </c>
       <c r="D56" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E56" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F56" t="s">
         <v>0</v>
@@ -2670,16 +2664,16 @@
         <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F57" t="s">
         <v>0</v>
@@ -2693,16 +2687,16 @@
         <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C58" t="s">
         <v>33</v>
       </c>
       <c r="D58" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E58" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F58" t="s">
         <v>0</v>
@@ -2716,16 +2710,16 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
         <v>33</v>
       </c>
       <c r="D59" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E59" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F59" t="s">
         <v>0</v>
@@ -2739,16 +2733,16 @@
         <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
         <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="E60" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
       <c r="F60" t="s">
         <v>0</v>
@@ -2762,16 +2756,16 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
         <v>33</v>
       </c>
       <c r="D61" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E61" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F61" t="s">
         <v>0</v>
@@ -2785,16 +2779,16 @@
         <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C62" t="s">
         <v>33</v>
       </c>
       <c r="D62" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E62" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F62" t="s">
         <v>0</v>
@@ -2808,16 +2802,16 @@
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C63" t="s">
         <v>33</v>
       </c>
       <c r="D63" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E63" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F63" t="s">
         <v>0</v>
@@ -2831,16 +2825,16 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C64" t="s">
         <v>33</v>
       </c>
       <c r="D64" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="E64" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="F64" t="s">
         <v>0</v>
@@ -2854,16 +2848,16 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C65" t="s">
         <v>33</v>
       </c>
       <c r="D65" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="E65" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="F65" t="s">
         <v>0</v>
@@ -2877,16 +2871,16 @@
         <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C66" t="s">
         <v>33</v>
       </c>
       <c r="D66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E66" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F66" t="s">
         <v>0</v>
@@ -2900,16 +2894,16 @@
         <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C67" t="s">
         <v>33</v>
       </c>
       <c r="D67" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E67" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F67" t="s">
         <v>0</v>
@@ -2923,16 +2917,13 @@
         <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" t="s">
-        <v>33</v>
+        <v>273</v>
       </c>
       <c r="D68" t="s">
-        <v>108</v>
+        <v>291</v>
       </c>
       <c r="E68" t="s">
-        <v>179</v>
+        <v>307</v>
       </c>
       <c r="F68" t="s">
         <v>0</v>
@@ -2946,13 +2937,16 @@
         <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>276</v>
+        <v>60</v>
+      </c>
+      <c r="C69" t="s">
+        <v>33</v>
       </c>
       <c r="D69" t="s">
-        <v>294</v>
+        <v>134</v>
       </c>
       <c r="E69" t="s">
-        <v>310</v>
+        <v>205</v>
       </c>
       <c r="F69" t="s">
         <v>0</v>
@@ -2966,16 +2960,16 @@
         <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>
       </c>
       <c r="D70" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="E70" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="F70" t="s">
         <v>0</v>
@@ -2989,16 +2983,16 @@
         <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C71" t="s">
         <v>33</v>
       </c>
       <c r="D71" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="E71" t="s">
-        <v>162</v>
+        <v>206</v>
       </c>
       <c r="F71" t="s">
         <v>0</v>
@@ -3012,16 +3006,16 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C72" t="s">
         <v>33</v>
       </c>
       <c r="D72" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E72" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F72" t="s">
         <v>0</v>
@@ -3035,16 +3029,16 @@
         <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C73" t="s">
         <v>33</v>
       </c>
       <c r="D73" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="E73" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="F73" t="s">
         <v>0</v>
@@ -3058,16 +3052,16 @@
         <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C74" t="s">
         <v>33</v>
       </c>
       <c r="D74" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E74" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F74" t="s">
         <v>0</v>
@@ -3081,16 +3075,16 @@
         <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C75" t="s">
         <v>33</v>
       </c>
       <c r="D75" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E75" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="F75" t="s">
         <v>0</v>
@@ -3104,16 +3098,16 @@
         <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C76" t="s">
         <v>33</v>
       </c>
       <c r="D76" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E76" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="F76" t="s">
         <v>0</v>
@@ -3127,16 +3121,16 @@
         <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C77" t="s">
         <v>33</v>
       </c>
       <c r="D77" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E77" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F77" t="s">
         <v>0</v>
@@ -3150,16 +3144,16 @@
         <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C78" t="s">
         <v>33</v>
       </c>
       <c r="D78" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E78" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F78" t="s">
         <v>0</v>
@@ -3173,16 +3167,16 @@
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C79" t="s">
         <v>33</v>
       </c>
       <c r="D79" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E79" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="F79" t="s">
         <v>0</v>
@@ -3196,16 +3190,16 @@
         <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C80" t="s">
         <v>33</v>
       </c>
       <c r="D80" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E80" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="F80" t="s">
         <v>0</v>
@@ -3219,16 +3213,16 @@
         <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C81" t="s">
         <v>33</v>
       </c>
       <c r="D81" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E81" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F81" t="s">
         <v>0</v>
@@ -3242,16 +3236,16 @@
         <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C82" t="s">
         <v>33</v>
       </c>
       <c r="D82" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E82" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F82" t="s">
         <v>0</v>
@@ -3265,16 +3259,16 @@
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C83" t="s">
         <v>33</v>
       </c>
       <c r="D83" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E83" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F83" t="s">
         <v>0</v>
@@ -3288,16 +3282,13 @@
         <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
-      </c>
-      <c r="C84" t="s">
-        <v>33</v>
+        <v>274</v>
       </c>
       <c r="D84" t="s">
-        <v>142</v>
+        <v>292</v>
       </c>
       <c r="E84" t="s">
-        <v>213</v>
+        <v>308</v>
       </c>
       <c r="F84" t="s">
         <v>0</v>
@@ -3311,13 +3302,13 @@
         <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
       <c r="D85" t="s">
-        <v>295</v>
+        <v>242</v>
       </c>
       <c r="E85" t="s">
-        <v>311</v>
+        <v>251</v>
       </c>
       <c r="F85" t="s">
         <v>0</v>
@@ -3331,13 +3322,16 @@
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>233</v>
+        <v>69</v>
+      </c>
+      <c r="C86" t="s">
+        <v>33</v>
       </c>
       <c r="D86" t="s">
-        <v>242</v>
+        <v>143</v>
       </c>
       <c r="E86" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="F86" t="s">
         <v>0</v>
@@ -3351,16 +3345,13 @@
         <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>69</v>
-      </c>
-      <c r="C87" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D87" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E87" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F87" t="s">
         <v>0</v>
@@ -3374,13 +3365,16 @@
         <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="C88" t="s">
+        <v>33</v>
       </c>
       <c r="D88" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E88" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F88" t="s">
         <v>0</v>
@@ -3394,16 +3388,13 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>66</v>
-      </c>
-      <c r="C89" t="s">
-        <v>33</v>
+        <v>234</v>
       </c>
       <c r="D89" t="s">
-        <v>140</v>
+        <v>243</v>
       </c>
       <c r="E89" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="F89" t="s">
         <v>0</v>
@@ -3417,13 +3408,16 @@
         <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>234</v>
+        <v>72</v>
+      </c>
+      <c r="C90" t="s">
+        <v>33</v>
       </c>
       <c r="D90" t="s">
-        <v>243</v>
+        <v>146</v>
       </c>
       <c r="E90" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="F90" t="s">
         <v>0</v>
@@ -3437,16 +3431,13 @@
         <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
-      </c>
-      <c r="C91" t="s">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="D91" t="s">
-        <v>146</v>
+        <v>293</v>
       </c>
       <c r="E91" t="s">
-        <v>217</v>
+        <v>309</v>
       </c>
       <c r="F91" t="s">
         <v>0</v>
@@ -3460,13 +3451,16 @@
         <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>278</v>
+        <v>73</v>
+      </c>
+      <c r="C92" t="s">
+        <v>33</v>
       </c>
       <c r="D92" t="s">
-        <v>296</v>
+        <v>147</v>
       </c>
       <c r="E92" t="s">
-        <v>312</v>
+        <v>218</v>
       </c>
       <c r="F92" t="s">
         <v>0</v>
@@ -3480,16 +3474,16 @@
         <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C93" t="s">
         <v>33</v>
       </c>
       <c r="D93" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E93" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F93" t="s">
         <v>0</v>
@@ -3503,16 +3497,16 @@
         <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C94" t="s">
         <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E94" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F94" t="s">
         <v>0</v>
@@ -3526,16 +3520,16 @@
         <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C95" t="s">
         <v>33</v>
       </c>
       <c r="D95" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E95" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F95" t="s">
         <v>0</v>
@@ -3549,16 +3543,13 @@
         <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
-      </c>
-      <c r="C96" t="s">
-        <v>33</v>
+        <v>235</v>
       </c>
       <c r="D96" t="s">
-        <v>151</v>
+        <v>244</v>
       </c>
       <c r="E96" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="F96" t="s">
         <v>0</v>
@@ -3572,13 +3563,13 @@
         <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c r="D97" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
       <c r="E97" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="F97" t="s">
         <v>0</v>
@@ -3592,13 +3583,16 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>279</v>
+        <v>49</v>
+      </c>
+      <c r="C98" t="s">
+        <v>81</v>
       </c>
       <c r="D98" t="s">
-        <v>297</v>
+        <v>123</v>
       </c>
       <c r="E98" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="F98" t="s">
         <v>0</v>
@@ -3612,16 +3606,16 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C99" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="D99" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="E99" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="F99" t="s">
         <v>0</v>
@@ -3635,16 +3629,16 @@
         <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C100" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="D100" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E100" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F100" t="s">
         <v>0</v>
@@ -3658,16 +3652,16 @@
         <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C101" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D101" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E101" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F101" t="s">
         <v>0</v>
@@ -3681,16 +3675,13 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>79</v>
-      </c>
-      <c r="C102" t="s">
-        <v>82</v>
+        <v>311</v>
       </c>
       <c r="D102" t="s">
-        <v>153</v>
+        <v>312</v>
       </c>
       <c r="E102" t="s">
-        <v>224</v>
+        <v>313</v>
       </c>
       <c r="F102" t="s">
         <v>0</v>
@@ -3879,32 +3870,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>8</v>
-      </c>
-      <c r="B112" t="s">
-        <v>341</v>
-      </c>
-      <c r="D112" t="s">
-        <v>342</v>
-      </c>
-      <c r="E112" t="s">
-        <v>343</v>
-      </c>
-      <c r="F112" t="s">
-        <v>0</v>
-      </c>
-      <c r="G112" t="s">
-        <v>226</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B113:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="B112:B1048576 B1">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B106 B2:B102">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="B105 B2:B101">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>